<commit_message>
Ya estan todas las tablas
</commit_message>
<xml_diff>
--- a/Output/Drive/1. Informacion Demografica.xlsx
+++ b/Output/Drive/1. Informacion Demografica.xlsx
@@ -23,13 +23,13 @@
     <t xml:space="preserve">Superficie (km2)</t>
   </si>
   <si>
-    <t xml:space="preserve">Densidad de Población (hab/km2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Población Urbana</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Población Rural</t>
+    <t xml:space="preserve">Densidad de población (hab./km2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Población Urbana%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Población Rural%</t>
   </si>
   <si>
     <t xml:space="preserve">Población total</t>
@@ -941,10 +941,10 @@
         <v>15</v>
       </c>
       <c r="C2" t="n">
-        <v>241.626989398186</v>
+        <v>241.60395471</v>
       </c>
       <c r="D2" t="n">
-        <v>92.15857903731</v>
+        <v>92.1673654999916</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
@@ -985,10 +985,10 @@
         <v>17</v>
       </c>
       <c r="C3" t="n">
-        <v>238.9</v>
+        <v>238.8680859</v>
       </c>
       <c r="D3" t="n">
-        <v>192.82126412725</v>
+        <v>192.847026116686</v>
       </c>
       <c r="E3" t="n">
         <v>42.8937371106046</v>
@@ -1029,10 +1029,10 @@
         <v>19</v>
       </c>
       <c r="C4" t="n">
-        <v>271.8</v>
+        <v>271.80287393</v>
       </c>
       <c r="D4" t="n">
-        <v>224.437086092715</v>
+        <v>224.434712988761</v>
       </c>
       <c r="E4" t="n">
         <v>73.2418609225927</v>
@@ -1073,10 +1073,10 @@
         <v>21</v>
       </c>
       <c r="C5" t="n">
-        <v>120</v>
+        <v>120.01906514</v>
       </c>
       <c r="D5" t="n">
-        <v>85.9416666666667</v>
+        <v>85.9280147530734</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -1117,10 +1117,10 @@
         <v>23</v>
       </c>
       <c r="C6" t="n">
-        <v>239</v>
+        <v>238.99099886</v>
       </c>
       <c r="D6" t="n">
-        <v>78.9623430962343</v>
+        <v>78.9653170622344</v>
       </c>
       <c r="E6" t="n">
         <v>67.8889359898262</v>
@@ -1161,10 +1161,10 @@
         <v>25</v>
       </c>
       <c r="C7" t="n">
-        <v>433.5</v>
+        <v>433.52336674</v>
       </c>
       <c r="D7" t="n">
-        <v>44.2029988465975</v>
+        <v>44.2006163222389</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
@@ -1205,10 +1205,10 @@
         <v>27</v>
       </c>
       <c r="C8" t="n">
-        <v>272.3</v>
+        <v>272.31966558</v>
       </c>
       <c r="D8" t="n">
-        <v>46.0741828865222</v>
+        <v>46.070855636808</v>
       </c>
       <c r="E8" t="n">
         <v>44.7792124980073</v>
@@ -1249,10 +1249,10 @@
         <v>29</v>
       </c>
       <c r="C9" t="n">
-        <v>322.2</v>
+        <v>322.22397435</v>
       </c>
       <c r="D9" t="n">
-        <v>144.882060831782</v>
+        <v>144.871281207943</v>
       </c>
       <c r="E9" t="n">
         <v>73.7837664146012</v>
@@ -1293,10 +1293,10 @@
         <v>31</v>
       </c>
       <c r="C10" t="n">
-        <v>137.6</v>
+        <v>137.59729501</v>
       </c>
       <c r="D10" t="n">
-        <v>144.156976744186</v>
+        <v>144.15981068929</v>
       </c>
       <c r="E10" t="n">
         <v>31.5083686227062</v>
@@ -1337,10 +1337,10 @@
         <v>33</v>
       </c>
       <c r="C11" t="n">
-        <v>62.5</v>
+        <v>62.45009249</v>
       </c>
       <c r="D11" t="n">
-        <v>504.4</v>
+        <v>504.803095448546</v>
       </c>
       <c r="E11" t="n">
         <v>92.3172085646312</v>
@@ -1381,10 +1381,10 @@
         <v>35</v>
       </c>
       <c r="C12" t="n">
-        <v>142.6</v>
+        <v>142.64968673</v>
       </c>
       <c r="D12" t="n">
-        <v>138.934081346424</v>
+        <v>138.885688809812</v>
       </c>
       <c r="E12" t="n">
         <v>14.9404401372905</v>
@@ -1425,10 +1425,10 @@
         <v>37</v>
       </c>
       <c r="C13" t="n">
-        <v>458.5</v>
+        <v>458.51095916</v>
       </c>
       <c r="D13" t="n">
-        <v>65.7251908396947</v>
+        <v>65.7236199004007</v>
       </c>
       <c r="E13" t="n">
         <v>27.9309772689564</v>
@@ -1469,10 +1469,10 @@
         <v>39</v>
       </c>
       <c r="C14" t="n">
-        <v>122.3</v>
+        <v>122.32060282</v>
       </c>
       <c r="D14" t="n">
-        <v>510.7931316435</v>
+        <v>510.707097249408</v>
       </c>
       <c r="E14" t="n">
         <v>76.2349927965424</v>
@@ -1513,10 +1513,10 @@
         <v>41</v>
       </c>
       <c r="C15" t="n">
-        <v>211</v>
+        <v>211.0101449</v>
       </c>
       <c r="D15" t="n">
-        <v>76.5402843601896</v>
+        <v>76.5366044729919</v>
       </c>
       <c r="E15" t="n">
         <v>26.2229102167183</v>
@@ -1557,10 +1557,10 @@
         <v>43</v>
       </c>
       <c r="C16" t="n">
-        <v>593.6</v>
+        <v>593.62836729</v>
       </c>
       <c r="D16" t="n">
-        <v>32.7341644204852</v>
+        <v>32.7326001766144</v>
       </c>
       <c r="E16" t="n">
         <v>0</v>
@@ -1601,10 +1601,10 @@
         <v>45</v>
       </c>
       <c r="C17" t="n">
-        <v>391.4</v>
+        <v>391.39363559</v>
       </c>
       <c r="D17" t="n">
-        <v>154.371486969852</v>
+        <v>154.373997188072</v>
       </c>
       <c r="E17" t="n">
         <v>49.0458615382069</v>
@@ -1645,10 +1645,10 @@
         <v>47</v>
       </c>
       <c r="C18" t="n">
-        <v>278.3</v>
+        <v>278.33061647</v>
       </c>
       <c r="D18" t="n">
-        <v>46.5936040244341</v>
+        <v>46.5884787108847</v>
       </c>
       <c r="E18" t="n">
         <v>0</v>
@@ -1689,10 +1689,10 @@
         <v>49</v>
       </c>
       <c r="C19" t="n">
-        <v>231.6</v>
+        <v>231.63244062</v>
       </c>
       <c r="D19" t="n">
-        <v>98.8903281519862</v>
+        <v>98.8764783494772</v>
       </c>
       <c r="E19" t="n">
         <v>17.700737894599</v>
@@ -1733,10 +1733,10 @@
         <v>51</v>
       </c>
       <c r="C20" t="n">
-        <v>222.8</v>
+        <v>222.82416015</v>
       </c>
       <c r="D20" t="n">
-        <v>84.8698384201077</v>
+        <v>84.8606362401227</v>
       </c>
       <c r="E20" t="n">
         <v>13.2846792532656</v>
@@ -1777,10 +1777,10 @@
         <v>53</v>
       </c>
       <c r="C21" t="n">
-        <v>239.5</v>
+        <v>239.53867876</v>
       </c>
       <c r="D21" t="n">
-        <v>10.8267223382046</v>
+        <v>10.8249741270302</v>
       </c>
       <c r="E21" t="n">
         <v>0</v>
@@ -1821,10 +1821,10 @@
         <v>55</v>
       </c>
       <c r="C22" t="n">
-        <v>123</v>
+        <v>123.01188621</v>
       </c>
       <c r="D22" t="n">
-        <v>123.373983739837</v>
+        <v>123.362062541615</v>
       </c>
       <c r="E22" t="n">
         <v>63.1565074135091</v>
@@ -1865,10 +1865,10 @@
         <v>57</v>
       </c>
       <c r="C23" t="n">
-        <v>142.3</v>
+        <v>142.33870812</v>
       </c>
       <c r="D23" t="n">
-        <v>114.441321152495</v>
+        <v>114.410199552119</v>
       </c>
       <c r="E23" t="n">
         <v>20.3254528707399</v>
@@ -1909,10 +1909,10 @@
         <v>59</v>
       </c>
       <c r="C24" t="n">
-        <v>98</v>
+        <v>98.03504701</v>
       </c>
       <c r="D24" t="n">
-        <v>369.877551020408</v>
+        <v>369.745321755214</v>
       </c>
       <c r="E24" t="n">
         <v>58.4611564775988</v>
@@ -1953,10 +1953,10 @@
         <v>61</v>
       </c>
       <c r="C25" t="n">
-        <v>302.8</v>
+        <v>302.84595862</v>
       </c>
       <c r="D25" t="n">
-        <v>58.1472919418758</v>
+        <v>58.138467755129</v>
       </c>
       <c r="E25" t="n">
         <v>0</v>
@@ -1997,10 +1997,10 @@
         <v>63</v>
       </c>
       <c r="C26" t="n">
-        <v>292.306140741408</v>
+        <v>292.31124081</v>
       </c>
       <c r="D26" t="n">
-        <v>70.7237964538303</v>
+        <v>70.7225625080812</v>
       </c>
       <c r="E26" t="n">
         <v>18.4104871087892</v>
@@ -2041,10 +2041,10 @@
         <v>65</v>
       </c>
       <c r="C27" t="n">
-        <v>107.5</v>
+        <v>107.45597616</v>
       </c>
       <c r="D27" t="n">
-        <v>118.753488372093</v>
+        <v>118.802140711017</v>
       </c>
       <c r="E27" t="n">
         <v>0</v>
@@ -2085,10 +2085,10 @@
         <v>67</v>
       </c>
       <c r="C28" t="n">
-        <v>213.9</v>
+        <v>213.91803679</v>
       </c>
       <c r="D28" t="n">
-        <v>106.806919121085</v>
+        <v>106.797913550542</v>
       </c>
       <c r="E28" t="n">
         <v>13.1007616212904</v>
@@ -2129,10 +2129,10 @@
         <v>69</v>
       </c>
       <c r="C29" t="n">
-        <v>394</v>
+        <v>394.04540566</v>
       </c>
       <c r="D29" t="n">
-        <v>321.779187817259</v>
+        <v>321.742109358312</v>
       </c>
       <c r="E29" t="n">
         <v>43.078221500067</v>
@@ -2173,10 +2173,10 @@
         <v>71</v>
       </c>
       <c r="C30" t="n">
-        <v>660.7</v>
+        <v>660.7457791</v>
       </c>
       <c r="D30" t="n">
-        <v>71.779930376873</v>
+        <v>71.7749571773239</v>
       </c>
       <c r="E30" t="n">
         <v>35.5888244596732</v>
@@ -2217,10 +2217,10 @@
         <v>73</v>
       </c>
       <c r="C31" t="n">
-        <v>486.6</v>
+        <v>486.59532185</v>
       </c>
       <c r="D31" t="n">
-        <v>202.741471434443</v>
+        <v>202.743420600356</v>
       </c>
       <c r="E31" t="n">
         <v>45.3423074583899</v>
@@ -2261,10 +2261,10 @@
         <v>75</v>
       </c>
       <c r="C32" t="n">
-        <v>441</v>
+        <v>440.98587366</v>
       </c>
       <c r="D32" t="n">
-        <v>27.8684807256236</v>
+        <v>27.8693734518026</v>
       </c>
       <c r="E32" t="n">
         <v>37.2823433685924</v>
@@ -2305,10 +2305,10 @@
         <v>77</v>
       </c>
       <c r="C33" t="n">
-        <v>38.3779353829223</v>
+        <v>38.38517377</v>
       </c>
       <c r="D33" t="n">
-        <v>274.194010047831</v>
+        <v>274.14230460575</v>
       </c>
       <c r="E33" t="n">
         <v>56.2482181887295</v>
@@ -2349,10 +2349,10 @@
         <v>79</v>
       </c>
       <c r="C34" t="n">
-        <v>110.8</v>
+        <v>110.7903024</v>
       </c>
       <c r="D34" t="n">
-        <v>26.1281588447653</v>
+        <v>26.1304458719484</v>
       </c>
       <c r="E34" t="n">
         <v>0</v>
@@ -2393,10 +2393,10 @@
         <v>81</v>
       </c>
       <c r="C35" t="n">
-        <v>177.2</v>
+        <v>177.20877914</v>
       </c>
       <c r="D35" t="n">
-        <v>53.4650112866817</v>
+        <v>53.4623625645277</v>
       </c>
       <c r="E35" t="n">
         <v>0</v>
@@ -2437,10 +2437,10 @@
         <v>83</v>
       </c>
       <c r="C36" t="n">
-        <v>146.3</v>
+        <v>146.3403203</v>
       </c>
       <c r="D36" t="n">
-        <v>89.3916609706083</v>
+        <v>89.3670314045363</v>
       </c>
       <c r="E36" t="n">
         <v>0</v>
@@ -2481,10 +2481,10 @@
         <v>85</v>
       </c>
       <c r="C37" t="n">
-        <v>245.7</v>
+        <v>245.72337691</v>
       </c>
       <c r="D37" t="n">
-        <v>38.4574684574685</v>
+        <v>38.4538098036185</v>
       </c>
       <c r="E37" t="n">
         <v>0</v>
@@ -2525,10 +2525,10 @@
         <v>87</v>
       </c>
       <c r="C38" t="n">
-        <v>796.9</v>
+        <v>796.90977735</v>
       </c>
       <c r="D38" t="n">
-        <v>26.3044296649517</v>
+        <v>26.3041069337935</v>
       </c>
       <c r="E38" t="n">
         <v>15.6187386699742</v>
@@ -2569,10 +2569,10 @@
         <v>89</v>
       </c>
       <c r="C39" t="n">
-        <v>192.1</v>
+        <v>192.14150463</v>
       </c>
       <c r="D39" t="n">
-        <v>46.2155127537741</v>
+        <v>46.2055297063279</v>
       </c>
       <c r="E39" t="n">
         <v>0</v>
@@ -2613,10 +2613,10 @@
         <v>91</v>
       </c>
       <c r="C40" t="n">
-        <v>53.4</v>
+        <v>53.42708858</v>
       </c>
       <c r="D40" t="n">
-        <v>268.239700374532</v>
+        <v>268.103697594371</v>
       </c>
       <c r="E40" t="n">
         <v>77.8344037978218</v>
@@ -2657,10 +2657,10 @@
         <v>93</v>
       </c>
       <c r="C41" t="n">
-        <v>232.8</v>
+        <v>232.78663733</v>
       </c>
       <c r="D41" t="n">
-        <v>42.1778350515464</v>
+        <v>42.1802561891923</v>
       </c>
       <c r="E41" t="n">
         <v>0</v>
@@ -2701,10 +2701,10 @@
         <v>95</v>
       </c>
       <c r="C42" t="n">
-        <v>135.9</v>
+        <v>135.86509674</v>
       </c>
       <c r="D42" t="n">
-        <v>347.47608535688</v>
+        <v>347.56535072703</v>
       </c>
       <c r="E42" t="n">
         <v>65.4313667358435</v>
@@ -2745,10 +2745,10 @@
         <v>97</v>
       </c>
       <c r="C43" t="n">
-        <v>198.3</v>
+        <v>198.26577265</v>
       </c>
       <c r="D43" t="n">
-        <v>58.3862834089763</v>
+        <v>58.3963628479573</v>
       </c>
       <c r="E43" t="n">
         <v>43.1421661772327</v>
@@ -2789,10 +2789,10 @@
         <v>99</v>
       </c>
       <c r="C44" t="n">
-        <v>249.7</v>
+        <v>249.70425397</v>
       </c>
       <c r="D44" t="n">
-        <v>25.0901081297557</v>
+        <v>25.0896806938367</v>
       </c>
       <c r="E44" t="n">
         <v>0</v>
@@ -2833,10 +2833,10 @@
         <v>101</v>
       </c>
       <c r="C45" t="n">
-        <v>341.3</v>
+        <v>341.31490835</v>
       </c>
       <c r="D45" t="n">
-        <v>49.6571930852622</v>
+        <v>49.6550241005609</v>
       </c>
       <c r="E45" t="n">
         <v>0</v>
@@ -2877,10 +2877,10 @@
         <v>103</v>
       </c>
       <c r="C46" t="n">
-        <v>79.7</v>
+        <v>79.73465508</v>
       </c>
       <c r="D46" t="n">
-        <v>116.624843161857</v>
+        <v>116.574154496236</v>
       </c>
       <c r="E46" t="n">
         <v>0</v>
@@ -2921,10 +2921,10 @@
         <v>105</v>
       </c>
       <c r="C47" t="n">
-        <v>324</v>
+        <v>323.98772958</v>
       </c>
       <c r="D47" t="n">
-        <v>118.802469135802</v>
+        <v>118.806968553713</v>
       </c>
       <c r="E47" t="n">
         <v>39.2860854203471</v>
@@ -2965,10 +2965,10 @@
         <v>107</v>
       </c>
       <c r="C48" t="n">
-        <v>385.4</v>
+        <v>385.39864483</v>
       </c>
       <c r="D48" t="n">
-        <v>12.3196678775298</v>
+        <v>12.3197111969461</v>
       </c>
       <c r="E48" t="n">
         <v>0</v>
@@ -3009,10 +3009,10 @@
         <v>109</v>
       </c>
       <c r="C49" t="n">
-        <v>154</v>
+        <v>154.03052242</v>
       </c>
       <c r="D49" t="n">
-        <v>2041.11038961039</v>
+        <v>2040.70592673122</v>
       </c>
       <c r="E49" t="n">
         <v>97.3031613172102</v>
@@ -3053,10 +3053,10 @@
         <v>111</v>
       </c>
       <c r="C50" t="n">
-        <v>188.1</v>
+        <v>188.07657968</v>
       </c>
       <c r="D50" t="n">
-        <v>99.5374800637959</v>
+        <v>99.5498750129121</v>
       </c>
       <c r="E50" t="n">
         <v>0</v>
@@ -3097,10 +3097,10 @@
         <v>113</v>
       </c>
       <c r="C51" t="n">
-        <v>91</v>
+        <v>90.97783726</v>
       </c>
       <c r="D51" t="n">
-        <v>259.791208791209</v>
+        <v>259.854495468362</v>
       </c>
       <c r="E51" t="n">
         <v>86.2273169493676</v>
@@ -3141,10 +3141,10 @@
         <v>115</v>
       </c>
       <c r="C52" t="n">
-        <v>112.5</v>
+        <v>112.53583047</v>
       </c>
       <c r="D52" t="n">
-        <v>1802.21333333333</v>
+        <v>1801.63952363642</v>
       </c>
       <c r="E52" t="n">
         <v>68.0121726864251</v>
@@ -3185,10 +3185,10 @@
         <v>117</v>
       </c>
       <c r="C53" t="n">
-        <v>297.4</v>
+        <v>297.36447474</v>
       </c>
       <c r="D53" t="n">
-        <v>130.77000672495</v>
+        <v>130.785629433389</v>
       </c>
       <c r="E53" t="n">
         <v>46.1314957188038</v>
@@ -3229,10 +3229,10 @@
         <v>119</v>
       </c>
       <c r="C54" t="n">
-        <v>359.4</v>
+        <v>359.39863319</v>
       </c>
       <c r="D54" t="n">
-        <v>49.2459654980523</v>
+        <v>49.2461527827882</v>
       </c>
       <c r="E54" t="n">
         <v>15.6167015085598</v>
@@ -3273,10 +3273,10 @@
         <v>121</v>
       </c>
       <c r="C55" t="n">
-        <v>205.7</v>
+        <v>205.71492716</v>
       </c>
       <c r="D55" t="n">
-        <v>178.881866796305</v>
+        <v>178.868886706413</v>
       </c>
       <c r="E55" t="n">
         <v>18.1976301771932</v>
@@ -3317,10 +3317,10 @@
         <v>123</v>
       </c>
       <c r="C56" t="n">
-        <v>256.2</v>
+        <v>256.22499311</v>
       </c>
       <c r="D56" t="n">
-        <v>71.5417642466823</v>
+        <v>71.5347858049553</v>
       </c>
       <c r="E56" t="n">
         <v>28.6649571716951</v>
@@ -3361,10 +3361,10 @@
         <v>125</v>
       </c>
       <c r="C57" t="n">
-        <v>64.3</v>
+        <v>64.29112174</v>
       </c>
       <c r="D57" t="n">
-        <v>615.256609642302</v>
+        <v>615.341573288903</v>
       </c>
       <c r="E57" t="n">
         <v>0</v>
@@ -3405,10 +3405,10 @@
         <v>127</v>
       </c>
       <c r="C58" t="n">
-        <v>420.2</v>
+        <v>420.20742226</v>
       </c>
       <c r="D58" t="n">
-        <v>36.0352213231794</v>
+        <v>36.0345848213766</v>
       </c>
       <c r="E58" t="n">
         <v>31.7329282789592</v>
@@ -3449,10 +3449,10 @@
         <v>129</v>
       </c>
       <c r="C59" t="n">
-        <v>240</v>
+        <v>240.01201236</v>
       </c>
       <c r="D59" t="n">
-        <v>72.6708333333333</v>
+        <v>72.6671962311612</v>
       </c>
       <c r="E59" t="n">
         <v>23.1064732526805</v>
@@ -3493,10 +3493,10 @@
         <v>131</v>
       </c>
       <c r="C60" t="n">
-        <v>525</v>
+        <v>525.02869222</v>
       </c>
       <c r="D60" t="n">
-        <v>72.4</v>
+        <v>72.3960434224666</v>
       </c>
       <c r="E60" t="n">
         <v>24.3646408839779</v>
@@ -3537,10 +3537,10 @@
         <v>133</v>
       </c>
       <c r="C61" t="n">
-        <v>176.643100601936</v>
+        <v>176.63193089</v>
       </c>
       <c r="D61" t="n">
-        <v>99.0868023735775</v>
+        <v>99.0930683473094</v>
       </c>
       <c r="E61" t="n">
         <v>14.9345826429755</v>
@@ -3581,10 +3581,10 @@
         <v>135</v>
       </c>
       <c r="C62" t="n">
-        <v>242.9</v>
+        <v>242.90861996</v>
       </c>
       <c r="D62" t="n">
-        <v>231.556195965418</v>
+        <v>231.547978862429</v>
       </c>
       <c r="E62" t="n">
         <v>85.5276024535514</v>
@@ -3625,10 +3625,10 @@
         <v>137</v>
       </c>
       <c r="C63" t="n">
-        <v>347.3</v>
+        <v>347.34481951</v>
       </c>
       <c r="D63" t="n">
-        <v>89.9366541894616</v>
+        <v>89.9250492466342</v>
       </c>
       <c r="E63" t="n">
         <v>0</v>
@@ -3669,10 +3669,10 @@
         <v>139</v>
       </c>
       <c r="C64" t="n">
-        <v>353.4</v>
+        <v>353.42541861</v>
       </c>
       <c r="D64" t="n">
-        <v>256.213921901528</v>
+        <v>256.195494812206</v>
       </c>
       <c r="E64" t="n">
         <v>72.8403242550748</v>
@@ -3713,10 +3713,10 @@
         <v>141</v>
       </c>
       <c r="C65" t="n">
-        <v>147.8</v>
+        <v>147.84988622</v>
       </c>
       <c r="D65" t="n">
-        <v>73.2746955345061</v>
+        <v>73.2499718253757</v>
       </c>
       <c r="E65" t="n">
         <v>0</v>
@@ -3757,10 +3757,10 @@
         <v>143</v>
       </c>
       <c r="C66" t="n">
-        <v>44.941882796785</v>
+        <v>44.93408666</v>
       </c>
       <c r="D66" t="n">
-        <v>261.849287739272</v>
+        <v>261.894719014636</v>
       </c>
       <c r="E66" t="n">
         <v>77.7107409925221</v>
@@ -3801,10 +3801,10 @@
         <v>145</v>
       </c>
       <c r="C67" t="n">
-        <v>90.7</v>
+        <v>90.72783863</v>
       </c>
       <c r="D67" t="n">
-        <v>143.682469680265</v>
+        <v>143.638382626376</v>
       </c>
       <c r="E67" t="n">
         <v>68.8152240638429</v>
@@ -3845,10 +3845,10 @@
         <v>147</v>
       </c>
       <c r="C68" t="n">
-        <v>163.3</v>
+        <v>163.34435588</v>
       </c>
       <c r="D68" t="n">
-        <v>337.624004898959</v>
+        <v>337.532323678841</v>
       </c>
       <c r="E68" t="n">
         <v>65.6636558203649</v>
@@ -3889,10 +3889,10 @@
         <v>149</v>
       </c>
       <c r="C69" t="n">
-        <v>265.7</v>
+        <v>265.68034426</v>
       </c>
       <c r="D69" t="n">
-        <v>53.9706435829883</v>
+        <v>53.9746364750514</v>
       </c>
       <c r="E69" t="n">
         <v>0</v>
@@ -3933,10 +3933,10 @@
         <v>151</v>
       </c>
       <c r="C70" t="n">
-        <v>76.8</v>
+        <v>76.80893605</v>
       </c>
       <c r="D70" t="n">
-        <v>2191.43229166667</v>
+        <v>2191.17733762698</v>
       </c>
       <c r="E70" t="n">
         <v>94.4522346733848</v>
@@ -3977,10 +3977,10 @@
         <v>153</v>
       </c>
       <c r="C71" t="n">
-        <v>31.5</v>
+        <v>31.52423159</v>
       </c>
       <c r="D71" t="n">
-        <v>605.301587301587</v>
+        <v>604.836312839687</v>
       </c>
       <c r="E71" t="n">
         <v>85.0684428593906</v>
@@ -4021,10 +4021,10 @@
         <v>155</v>
       </c>
       <c r="C72" t="n">
-        <v>531.6</v>
+        <v>531.59848768</v>
       </c>
       <c r="D72" t="n">
-        <v>17.09179834462</v>
+        <v>17.0918469682882</v>
       </c>
       <c r="E72" t="n">
         <v>0</v>
@@ -4065,10 +4065,10 @@
         <v>157</v>
       </c>
       <c r="C73" t="n">
-        <v>82.9</v>
+        <v>82.92694023</v>
       </c>
       <c r="D73" t="n">
-        <v>134.053075995175</v>
+        <v>134.009526568541</v>
       </c>
       <c r="E73" t="n">
         <v>72.5456672365698</v>
@@ -4109,10 +4109,10 @@
         <v>159</v>
       </c>
       <c r="C74" t="n">
-        <v>392.1</v>
+        <v>392.11136348</v>
       </c>
       <c r="D74" t="n">
-        <v>96.2050497322112</v>
+        <v>96.2022616871292</v>
       </c>
       <c r="E74" t="n">
         <v>22.9812841312762</v>
@@ -4153,10 +4153,10 @@
         <v>161</v>
       </c>
       <c r="C75" t="n">
-        <v>39</v>
+        <v>38.98056924</v>
       </c>
       <c r="D75" t="n">
-        <v>734</v>
+        <v>734.365879157695</v>
       </c>
       <c r="E75" t="n">
         <v>95.3992873611402</v>
@@ -4197,10 +4197,10 @@
         <v>163</v>
       </c>
       <c r="C76" t="n">
-        <v>128.8</v>
+        <v>128.80692211</v>
       </c>
       <c r="D76" t="n">
-        <v>165.854037267081</v>
+        <v>165.845124237632</v>
       </c>
       <c r="E76" t="n">
         <v>78.1762007302687</v>
@@ -4241,10 +4241,10 @@
         <v>165</v>
       </c>
       <c r="C77" t="n">
-        <v>336.1</v>
+        <v>336.11244819</v>
       </c>
       <c r="D77" t="n">
-        <v>342.478429038976</v>
+        <v>342.465745079848</v>
       </c>
       <c r="E77" t="n">
         <v>69.0427167765644</v>
@@ -4285,10 +4285,10 @@
         <v>167</v>
       </c>
       <c r="C78" t="n">
-        <v>217.4</v>
+        <v>217.41467837</v>
       </c>
       <c r="D78" t="n">
-        <v>774.466421343146</v>
+        <v>774.414134603492</v>
       </c>
       <c r="E78" t="n">
         <v>86.7822144476376</v>
@@ -4329,10 +4329,10 @@
         <v>169</v>
       </c>
       <c r="C79" t="n">
-        <v>135.4</v>
+        <v>135.41019859</v>
       </c>
       <c r="D79" t="n">
-        <v>134.859675036928</v>
+        <v>134.849517910304</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
@@ -4373,10 +4373,10 @@
         <v>171</v>
       </c>
       <c r="C80" t="n">
-        <v>176.8</v>
+        <v>176.84300888</v>
       </c>
       <c r="D80" t="n">
-        <v>39.6776018099548</v>
+        <v>39.6679520690589</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
@@ -4417,10 +4417,10 @@
         <v>173</v>
       </c>
       <c r="C81" t="n">
-        <v>154.4</v>
+        <v>154.35402674</v>
       </c>
       <c r="D81" t="n">
-        <v>159.805699481865</v>
+        <v>159.853296484204</v>
       </c>
       <c r="E81" t="n">
         <v>20.0251276647483</v>
@@ -4461,10 +4461,10 @@
         <v>175</v>
       </c>
       <c r="C82" t="n">
-        <v>272.7</v>
+        <v>272.69200265</v>
       </c>
       <c r="D82" t="n">
-        <v>139.91565823249</v>
+        <v>139.919761596279</v>
       </c>
       <c r="E82" t="n">
         <v>77.2428253177827</v>
@@ -4505,10 +4505,10 @@
         <v>177</v>
       </c>
       <c r="C83" t="n">
-        <v>105.3</v>
+        <v>105.25738969</v>
       </c>
       <c r="D83" t="n">
-        <v>203.63722697056</v>
+        <v>203.719663418911</v>
       </c>
       <c r="E83" t="n">
         <v>98.7315207760108</v>
@@ -4549,10 +4549,10 @@
         <v>179</v>
       </c>
       <c r="C84" t="n">
-        <v>319.9</v>
+        <v>319.87990261</v>
       </c>
       <c r="D84" t="n">
-        <v>181.012816505158</v>
+        <v>181.024189164517</v>
       </c>
       <c r="E84" t="n">
         <v>60.6223880081511</v>
@@ -4593,10 +4593,10 @@
         <v>181</v>
       </c>
       <c r="C85" t="n">
-        <v>872.5</v>
+        <v>872.49980798</v>
       </c>
       <c r="D85" t="n">
-        <v>45.7616045845272</v>
+        <v>45.7616146557539</v>
       </c>
       <c r="E85" t="n">
         <v>36.8973376411952</v>

</xml_diff>

<commit_message>
Todas las bases homologadas para unirse
</commit_message>
<xml_diff>
--- a/Output/Drive/1. Informacion Demografica.xlsx
+++ b/Output/Drive/1. Informacion Demografica.xlsx
@@ -26,13 +26,13 @@
     <t xml:space="preserve">Densidad de población (hab./km2)</t>
   </si>
   <si>
-    <t xml:space="preserve">Población Urbana%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Población Rural%</t>
-  </si>
-  <si>
     <t xml:space="preserve">Población total</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Población Rural</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Población Urbana</t>
   </si>
   <si>
     <t xml:space="preserve">Población Mujeres</t>
@@ -947,13 +947,13 @@
         <v>92.1673654999916</v>
       </c>
       <c r="E2" t="n">
+        <v>22268</v>
+      </c>
+      <c r="F2" t="n">
+        <v>22268</v>
+      </c>
+      <c r="G2" t="n">
         <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>100</v>
-      </c>
-      <c r="G2" t="n">
-        <v>22268</v>
       </c>
       <c r="H2" t="n">
         <v>11563</v>
@@ -991,13 +991,13 @@
         <v>192.847026116686</v>
       </c>
       <c r="E3" t="n">
-        <v>42.8937371106046</v>
+        <v>46065</v>
       </c>
       <c r="F3" t="n">
-        <v>57.1344838814718</v>
+        <v>26306</v>
       </c>
       <c r="G3" t="n">
-        <v>46065</v>
+        <v>19759</v>
       </c>
       <c r="H3" t="n">
         <v>24348</v>
@@ -1035,13 +1035,13 @@
         <v>224.434712988761</v>
       </c>
       <c r="E4" t="n">
-        <v>73.2418609225927</v>
+        <v>61002</v>
       </c>
       <c r="F4" t="n">
-        <v>26.7581390774073</v>
+        <v>16323</v>
       </c>
       <c r="G4" t="n">
-        <v>61002</v>
+        <v>44679</v>
       </c>
       <c r="H4" t="n">
         <v>31925</v>
@@ -1079,13 +1079,13 @@
         <v>85.9280147530734</v>
       </c>
       <c r="E5" t="n">
+        <v>10313</v>
+      </c>
+      <c r="F5" t="n">
+        <v>10313</v>
+      </c>
+      <c r="G5" t="n">
         <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>100</v>
-      </c>
-      <c r="G5" t="n">
-        <v>10313</v>
       </c>
       <c r="H5" t="n">
         <v>5400</v>
@@ -1123,13 +1123,13 @@
         <v>78.9653170622344</v>
       </c>
       <c r="E6" t="n">
-        <v>67.8889359898262</v>
+        <v>18872</v>
       </c>
       <c r="F6" t="n">
-        <v>32.1110640101738</v>
+        <v>6060</v>
       </c>
       <c r="G6" t="n">
-        <v>18872</v>
+        <v>12812</v>
       </c>
       <c r="H6" t="n">
         <v>9764</v>
@@ -1167,13 +1167,13 @@
         <v>44.2006163222389</v>
       </c>
       <c r="E7" t="n">
+        <v>19162</v>
+      </c>
+      <c r="F7" t="n">
+        <v>19162</v>
+      </c>
+      <c r="G7" t="n">
         <v>0</v>
-      </c>
-      <c r="F7" t="n">
-        <v>100</v>
-      </c>
-      <c r="G7" t="n">
-        <v>19162</v>
       </c>
       <c r="H7" t="n">
         <v>9964</v>
@@ -1211,13 +1211,13 @@
         <v>46.070855636808</v>
       </c>
       <c r="E8" t="n">
-        <v>44.7792124980073</v>
+        <v>12546</v>
       </c>
       <c r="F8" t="n">
-        <v>55.2207875019927</v>
+        <v>6928</v>
       </c>
       <c r="G8" t="n">
-        <v>12546</v>
+        <v>5618</v>
       </c>
       <c r="H8" t="n">
         <v>6476</v>
@@ -1255,13 +1255,13 @@
         <v>144.871281207943</v>
       </c>
       <c r="E9" t="n">
-        <v>73.7837664146012</v>
+        <v>46681</v>
       </c>
       <c r="F9" t="n">
-        <v>26.2162335853988</v>
+        <v>12238</v>
       </c>
       <c r="G9" t="n">
-        <v>46681</v>
+        <v>34443</v>
       </c>
       <c r="H9" t="n">
         <v>24393</v>
@@ -1299,13 +1299,13 @@
         <v>144.15981068929</v>
       </c>
       <c r="E10" t="n">
-        <v>31.5083686227062</v>
+        <v>19836</v>
       </c>
       <c r="F10" t="n">
-        <v>68.4916313772938</v>
+        <v>13586</v>
       </c>
       <c r="G10" t="n">
-        <v>19836</v>
+        <v>6250</v>
       </c>
       <c r="H10" t="n">
         <v>10261</v>
@@ -1343,13 +1343,13 @@
         <v>504.803095448546</v>
       </c>
       <c r="E11" t="n">
-        <v>92.3172085646312</v>
+        <v>31525</v>
       </c>
       <c r="F11" t="n">
-        <v>7.68279143536876</v>
+        <v>2422</v>
       </c>
       <c r="G11" t="n">
-        <v>31525</v>
+        <v>29103</v>
       </c>
       <c r="H11" t="n">
         <v>16044</v>
@@ -1387,13 +1387,13 @@
         <v>138.885688809812</v>
       </c>
       <c r="E12" t="n">
-        <v>14.9404401372905</v>
+        <v>19812</v>
       </c>
       <c r="F12" t="n">
-        <v>85.0595598627095</v>
+        <v>16852</v>
       </c>
       <c r="G12" t="n">
-        <v>19812</v>
+        <v>2960</v>
       </c>
       <c r="H12" t="n">
         <v>10301</v>
@@ -1431,13 +1431,13 @@
         <v>65.7236199004007</v>
       </c>
       <c r="E13" t="n">
-        <v>27.9309772689564</v>
+        <v>30135</v>
       </c>
       <c r="F13" t="n">
-        <v>72.0690227310436</v>
+        <v>21718</v>
       </c>
       <c r="G13" t="n">
-        <v>30135</v>
+        <v>8417</v>
       </c>
       <c r="H13" t="n">
         <v>15874</v>
@@ -1475,13 +1475,13 @@
         <v>510.707097249408</v>
       </c>
       <c r="E14" t="n">
-        <v>76.2349927965424</v>
+        <v>62470</v>
       </c>
       <c r="F14" t="n">
-        <v>23.7602048983512</v>
+        <v>14846</v>
       </c>
       <c r="G14" t="n">
-        <v>62470</v>
+        <v>47624</v>
       </c>
       <c r="H14" t="n">
         <v>32056</v>
@@ -1519,13 +1519,13 @@
         <v>76.5366044729919</v>
       </c>
       <c r="E15" t="n">
-        <v>26.2229102167183</v>
+        <v>16150</v>
       </c>
       <c r="F15" t="n">
-        <v>73.7770897832817</v>
+        <v>11915</v>
       </c>
       <c r="G15" t="n">
-        <v>16150</v>
+        <v>4235</v>
       </c>
       <c r="H15" t="n">
         <v>8406</v>
@@ -1563,13 +1563,13 @@
         <v>32.7326001766144</v>
       </c>
       <c r="E16" t="n">
+        <v>19431</v>
+      </c>
+      <c r="F16" t="n">
+        <v>19431</v>
+      </c>
+      <c r="G16" t="n">
         <v>0</v>
-      </c>
-      <c r="F16" t="n">
-        <v>100</v>
-      </c>
-      <c r="G16" t="n">
-        <v>19431</v>
       </c>
       <c r="H16" t="n">
         <v>10123</v>
@@ -1607,13 +1607,13 @@
         <v>154.373997188072</v>
       </c>
       <c r="E17" t="n">
-        <v>49.0458615382069</v>
+        <v>60421</v>
       </c>
       <c r="F17" t="n">
-        <v>50.4559672961388</v>
+        <v>30787</v>
       </c>
       <c r="G17" t="n">
-        <v>60421</v>
+        <v>29634</v>
       </c>
       <c r="H17" t="n">
         <v>31555</v>
@@ -1651,13 +1651,13 @@
         <v>46.5884787108847</v>
       </c>
       <c r="E18" t="n">
+        <v>12967</v>
+      </c>
+      <c r="F18" t="n">
+        <v>12967</v>
+      </c>
+      <c r="G18" t="n">
         <v>0</v>
-      </c>
-      <c r="F18" t="n">
-        <v>100</v>
-      </c>
-      <c r="G18" t="n">
-        <v>12967</v>
       </c>
       <c r="H18" t="n">
         <v>6690</v>
@@ -1695,13 +1695,13 @@
         <v>98.8764783494772</v>
       </c>
       <c r="E19" t="n">
-        <v>17.700737894599</v>
+        <v>22903</v>
       </c>
       <c r="F19" t="n">
-        <v>82.299262105401</v>
+        <v>18849</v>
       </c>
       <c r="G19" t="n">
-        <v>22903</v>
+        <v>4054</v>
       </c>
       <c r="H19" t="n">
         <v>11641</v>
@@ -1739,13 +1739,13 @@
         <v>84.8606362401227</v>
       </c>
       <c r="E20" t="n">
-        <v>13.2846792532656</v>
+        <v>18909</v>
       </c>
       <c r="F20" t="n">
-        <v>86.7153207467344</v>
+        <v>16397</v>
       </c>
       <c r="G20" t="n">
-        <v>18909</v>
+        <v>2512</v>
       </c>
       <c r="H20" t="n">
         <v>9719</v>
@@ -1783,13 +1783,13 @@
         <v>10.8249741270302</v>
       </c>
       <c r="E21" t="n">
+        <v>2593</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2593</v>
+      </c>
+      <c r="G21" t="n">
         <v>0</v>
-      </c>
-      <c r="F21" t="n">
-        <v>100</v>
-      </c>
-      <c r="G21" t="n">
-        <v>2593</v>
       </c>
       <c r="H21" t="n">
         <v>1354</v>
@@ -1827,13 +1827,13 @@
         <v>123.362062541615</v>
       </c>
       <c r="E22" t="n">
-        <v>63.1565074135091</v>
+        <v>15175</v>
       </c>
       <c r="F22" t="n">
-        <v>36.8434925864909</v>
+        <v>5591</v>
       </c>
       <c r="G22" t="n">
-        <v>15175</v>
+        <v>9584</v>
       </c>
       <c r="H22" t="n">
         <v>7837</v>
@@ -1871,13 +1871,13 @@
         <v>114.410199552119</v>
       </c>
       <c r="E23" t="n">
-        <v>20.3254528707399</v>
+        <v>16285</v>
       </c>
       <c r="F23" t="n">
-        <v>79.67454712926</v>
+        <v>12975</v>
       </c>
       <c r="G23" t="n">
-        <v>16285</v>
+        <v>3310</v>
       </c>
       <c r="H23" t="n">
         <v>8406</v>
@@ -1915,13 +1915,13 @@
         <v>369.745321755214</v>
       </c>
       <c r="E24" t="n">
-        <v>58.4611564775988</v>
+        <v>36248</v>
       </c>
       <c r="F24" t="n">
-        <v>41.5388435224012</v>
+        <v>15057</v>
       </c>
       <c r="G24" t="n">
-        <v>36248</v>
+        <v>21191</v>
       </c>
       <c r="H24" t="n">
         <v>18952</v>
@@ -1959,13 +1959,13 @@
         <v>58.138467755129</v>
       </c>
       <c r="E25" t="n">
+        <v>17607</v>
+      </c>
+      <c r="F25" t="n">
+        <v>17607</v>
+      </c>
+      <c r="G25" t="n">
         <v>0</v>
-      </c>
-      <c r="F25" t="n">
-        <v>100</v>
-      </c>
-      <c r="G25" t="n">
-        <v>17607</v>
       </c>
       <c r="H25" t="n">
         <v>9288</v>
@@ -2003,13 +2003,13 @@
         <v>70.7225625080812</v>
       </c>
       <c r="E26" t="n">
-        <v>18.4104871087892</v>
+        <v>20673</v>
       </c>
       <c r="F26" t="n">
-        <v>81.5604895274029</v>
+        <v>16867</v>
       </c>
       <c r="G26" t="n">
-        <v>20673</v>
+        <v>3806</v>
       </c>
       <c r="H26" t="n">
         <v>10812</v>
@@ -2047,13 +2047,13 @@
         <v>118.802140711017</v>
       </c>
       <c r="E27" t="n">
+        <v>12766</v>
+      </c>
+      <c r="F27" t="n">
+        <v>12766</v>
+      </c>
+      <c r="G27" t="n">
         <v>0</v>
-      </c>
-      <c r="F27" t="n">
-        <v>100</v>
-      </c>
-      <c r="G27" t="n">
-        <v>12766</v>
       </c>
       <c r="H27" t="n">
         <v>6571</v>
@@ -2091,13 +2091,13 @@
         <v>106.797913550542</v>
       </c>
       <c r="E28" t="n">
-        <v>13.1007616212904</v>
+        <v>22846</v>
       </c>
       <c r="F28" t="n">
-        <v>86.8992383787096</v>
+        <v>19853</v>
       </c>
       <c r="G28" t="n">
-        <v>22846</v>
+        <v>2993</v>
       </c>
       <c r="H28" t="n">
         <v>11830</v>
@@ -2135,13 +2135,13 @@
         <v>321.742109358312</v>
       </c>
       <c r="E29" t="n">
-        <v>43.078221500067</v>
+        <v>126781</v>
       </c>
       <c r="F29" t="n">
-        <v>56.921778499933</v>
+        <v>72166</v>
       </c>
       <c r="G29" t="n">
-        <v>126781</v>
+        <v>54615</v>
       </c>
       <c r="H29" t="n">
         <v>65460</v>
@@ -2179,13 +2179,13 @@
         <v>71.7749571773239</v>
       </c>
       <c r="E30" t="n">
-        <v>35.5888244596732</v>
+        <v>47425</v>
       </c>
       <c r="F30" t="n">
-        <v>64.4111755403268</v>
+        <v>30547</v>
       </c>
       <c r="G30" t="n">
-        <v>47425</v>
+        <v>16878</v>
       </c>
       <c r="H30" t="n">
         <v>24645</v>
@@ -2223,13 +2223,13 @@
         <v>202.743420600356</v>
       </c>
       <c r="E31" t="n">
-        <v>45.3423074583899</v>
+        <v>98654</v>
       </c>
       <c r="F31" t="n">
-        <v>54.6576925416101</v>
+        <v>53922</v>
       </c>
       <c r="G31" t="n">
-        <v>98654</v>
+        <v>44732</v>
       </c>
       <c r="H31" t="n">
         <v>52214</v>
@@ -2267,13 +2267,13 @@
         <v>27.8693734518026</v>
       </c>
       <c r="E32" t="n">
-        <v>37.2823433685924</v>
+        <v>12290</v>
       </c>
       <c r="F32" t="n">
-        <v>62.7176566314077</v>
+        <v>7708</v>
       </c>
       <c r="G32" t="n">
-        <v>12290</v>
+        <v>4582</v>
       </c>
       <c r="H32" t="n">
         <v>6430</v>
@@ -2311,13 +2311,13 @@
         <v>274.14230460575</v>
       </c>
       <c r="E33" t="n">
-        <v>56.2482181887295</v>
+        <v>10523</v>
       </c>
       <c r="F33" t="n">
-        <v>43.7517818112706</v>
+        <v>4604</v>
       </c>
       <c r="G33" t="n">
-        <v>10523</v>
+        <v>5919</v>
       </c>
       <c r="H33" t="n">
         <v>5385</v>
@@ -2355,13 +2355,13 @@
         <v>26.1304458719484</v>
       </c>
       <c r="E34" t="n">
+        <v>2895</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2895</v>
+      </c>
+      <c r="G34" t="n">
         <v>0</v>
-      </c>
-      <c r="F34" t="n">
-        <v>100</v>
-      </c>
-      <c r="G34" t="n">
-        <v>2895</v>
       </c>
       <c r="H34" t="n">
         <v>1525</v>
@@ -2399,13 +2399,13 @@
         <v>53.4623625645277</v>
       </c>
       <c r="E35" t="n">
+        <v>9474</v>
+      </c>
+      <c r="F35" t="n">
+        <v>9474</v>
+      </c>
+      <c r="G35" t="n">
         <v>0</v>
-      </c>
-      <c r="F35" t="n">
-        <v>100</v>
-      </c>
-      <c r="G35" t="n">
-        <v>9474</v>
       </c>
       <c r="H35" t="n">
         <v>4897</v>
@@ -2443,13 +2443,13 @@
         <v>89.3670314045363</v>
       </c>
       <c r="E36" t="n">
+        <v>13078</v>
+      </c>
+      <c r="F36" t="n">
+        <v>13078</v>
+      </c>
+      <c r="G36" t="n">
         <v>0</v>
-      </c>
-      <c r="F36" t="n">
-        <v>100</v>
-      </c>
-      <c r="G36" t="n">
-        <v>13078</v>
       </c>
       <c r="H36" t="n">
         <v>6893</v>
@@ -2487,13 +2487,13 @@
         <v>38.4538098036185</v>
       </c>
       <c r="E37" t="n">
+        <v>9449</v>
+      </c>
+      <c r="F37" t="n">
+        <v>9449</v>
+      </c>
+      <c r="G37" t="n">
         <v>0</v>
-      </c>
-      <c r="F37" t="n">
-        <v>100</v>
-      </c>
-      <c r="G37" t="n">
-        <v>9449</v>
       </c>
       <c r="H37" t="n">
         <v>4867</v>
@@ -2531,13 +2531,13 @@
         <v>26.3041069337935</v>
       </c>
       <c r="E38" t="n">
-        <v>15.6187386699742</v>
+        <v>20962</v>
       </c>
       <c r="F38" t="n">
-        <v>84.3812613300258</v>
+        <v>17688</v>
       </c>
       <c r="G38" t="n">
-        <v>20962</v>
+        <v>3274</v>
       </c>
       <c r="H38" t="n">
         <v>10888</v>
@@ -2575,13 +2575,13 @@
         <v>46.2055297063279</v>
       </c>
       <c r="E39" t="n">
+        <v>8878</v>
+      </c>
+      <c r="F39" t="n">
+        <v>8878</v>
+      </c>
+      <c r="G39" t="n">
         <v>0</v>
-      </c>
-      <c r="F39" t="n">
-        <v>100</v>
-      </c>
-      <c r="G39" t="n">
-        <v>8878</v>
       </c>
       <c r="H39" t="n">
         <v>4577</v>
@@ -2619,13 +2619,13 @@
         <v>268.103697594371</v>
       </c>
       <c r="E40" t="n">
-        <v>77.8344037978218</v>
+        <v>14324</v>
       </c>
       <c r="F40" t="n">
-        <v>22.1655962021782</v>
+        <v>3175</v>
       </c>
       <c r="G40" t="n">
-        <v>14324</v>
+        <v>11149</v>
       </c>
       <c r="H40" t="n">
         <v>7507</v>
@@ -2663,13 +2663,13 @@
         <v>42.1802561891923</v>
       </c>
       <c r="E41" t="n">
+        <v>9819</v>
+      </c>
+      <c r="F41" t="n">
+        <v>9819</v>
+      </c>
+      <c r="G41" t="n">
         <v>0</v>
-      </c>
-      <c r="F41" t="n">
-        <v>100</v>
-      </c>
-      <c r="G41" t="n">
-        <v>9819</v>
       </c>
       <c r="H41" t="n">
         <v>5062</v>
@@ -2707,13 +2707,13 @@
         <v>347.56535072703</v>
       </c>
       <c r="E42" t="n">
-        <v>65.4313667358435</v>
+        <v>47222</v>
       </c>
       <c r="F42" t="n">
-        <v>34.5686332641565</v>
+        <v>16324</v>
       </c>
       <c r="G42" t="n">
-        <v>47222</v>
+        <v>30898</v>
       </c>
       <c r="H42" t="n">
         <v>24597</v>
@@ -2751,13 +2751,13 @@
         <v>58.3963628479573</v>
       </c>
       <c r="E43" t="n">
-        <v>43.1421661772327</v>
+        <v>11578</v>
       </c>
       <c r="F43" t="n">
-        <v>56.8578338227673</v>
+        <v>6583</v>
       </c>
       <c r="G43" t="n">
-        <v>11578</v>
+        <v>4995</v>
       </c>
       <c r="H43" t="n">
         <v>5893</v>
@@ -2795,13 +2795,13 @@
         <v>25.0896806938367</v>
       </c>
       <c r="E44" t="n">
+        <v>6265</v>
+      </c>
+      <c r="F44" t="n">
+        <v>6265</v>
+      </c>
+      <c r="G44" t="n">
         <v>0</v>
-      </c>
-      <c r="F44" t="n">
-        <v>100</v>
-      </c>
-      <c r="G44" t="n">
-        <v>6265</v>
       </c>
       <c r="H44" t="n">
         <v>3229</v>
@@ -2839,13 +2839,13 @@
         <v>49.6550241005609</v>
       </c>
       <c r="E45" t="n">
+        <v>16948</v>
+      </c>
+      <c r="F45" t="n">
+        <v>16948</v>
+      </c>
+      <c r="G45" t="n">
         <v>0</v>
-      </c>
-      <c r="F45" t="n">
-        <v>100</v>
-      </c>
-      <c r="G45" t="n">
-        <v>16948</v>
       </c>
       <c r="H45" t="n">
         <v>8711</v>
@@ -2883,13 +2883,13 @@
         <v>116.574154496236</v>
       </c>
       <c r="E46" t="n">
+        <v>9295</v>
+      </c>
+      <c r="F46" t="n">
+        <v>9295</v>
+      </c>
+      <c r="G46" t="n">
         <v>0</v>
-      </c>
-      <c r="F46" t="n">
-        <v>100</v>
-      </c>
-      <c r="G46" t="n">
-        <v>9295</v>
       </c>
       <c r="H46" t="n">
         <v>4873</v>
@@ -2927,13 +2927,13 @@
         <v>118.806968553713</v>
       </c>
       <c r="E47" t="n">
-        <v>39.2860854203471</v>
+        <v>38492</v>
       </c>
       <c r="F47" t="n">
-        <v>61.5088849631092</v>
+        <v>23370</v>
       </c>
       <c r="G47" t="n">
-        <v>38492</v>
+        <v>15122</v>
       </c>
       <c r="H47" t="n">
         <v>19764</v>
@@ -2971,13 +2971,13 @@
         <v>12.3197111969461</v>
       </c>
       <c r="E48" t="n">
+        <v>4748</v>
+      </c>
+      <c r="F48" t="n">
+        <v>4748</v>
+      </c>
+      <c r="G48" t="n">
         <v>0</v>
-      </c>
-      <c r="F48" t="n">
-        <v>100</v>
-      </c>
-      <c r="G48" t="n">
-        <v>4748</v>
       </c>
       <c r="H48" t="n">
         <v>2518</v>
@@ -3015,13 +3015,13 @@
         <v>2040.70592673122</v>
       </c>
       <c r="E49" t="n">
-        <v>97.3031613172102</v>
+        <v>314331</v>
       </c>
       <c r="F49" t="n">
-        <v>2.6968386827898</v>
+        <v>8477</v>
       </c>
       <c r="G49" t="n">
-        <v>314331</v>
+        <v>305854</v>
       </c>
       <c r="H49" t="n">
         <v>164772</v>
@@ -3059,13 +3059,13 @@
         <v>99.5498750129121</v>
       </c>
       <c r="E50" t="n">
+        <v>18723</v>
+      </c>
+      <c r="F50" t="n">
+        <v>18723</v>
+      </c>
+      <c r="G50" t="n">
         <v>0</v>
-      </c>
-      <c r="F50" t="n">
-        <v>100</v>
-      </c>
-      <c r="G50" t="n">
-        <v>18723</v>
       </c>
       <c r="H50" t="n">
         <v>9614</v>
@@ -3103,13 +3103,13 @@
         <v>259.854495468362</v>
       </c>
       <c r="E51" t="n">
-        <v>86.2273169493676</v>
+        <v>23641</v>
       </c>
       <c r="F51" t="n">
-        <v>13.7726830506324</v>
+        <v>3256</v>
       </c>
       <c r="G51" t="n">
-        <v>23641</v>
+        <v>20385</v>
       </c>
       <c r="H51" t="n">
         <v>12476</v>
@@ -3147,13 +3147,13 @@
         <v>1801.63952363642</v>
       </c>
       <c r="E52" t="n">
-        <v>68.0121726864251</v>
+        <v>202749</v>
       </c>
       <c r="F52" t="n">
-        <v>31.9878273135749</v>
+        <v>64855</v>
       </c>
       <c r="G52" t="n">
-        <v>202749</v>
+        <v>137894</v>
       </c>
       <c r="H52" t="n">
         <v>106490</v>
@@ -3191,13 +3191,13 @@
         <v>130.785629433389</v>
       </c>
       <c r="E53" t="n">
-        <v>46.1314957188038</v>
+        <v>38891</v>
       </c>
       <c r="F53" t="n">
-        <v>53.8685042811962</v>
+        <v>20950</v>
       </c>
       <c r="G53" t="n">
-        <v>38891</v>
+        <v>17941</v>
       </c>
       <c r="H53" t="n">
         <v>19941</v>
@@ -3235,13 +3235,13 @@
         <v>49.2461527827882</v>
       </c>
       <c r="E54" t="n">
-        <v>15.6167015085598</v>
+        <v>17699</v>
       </c>
       <c r="F54" t="n">
-        <v>84.3832984914402</v>
+        <v>14935</v>
       </c>
       <c r="G54" t="n">
-        <v>17699</v>
+        <v>2764</v>
       </c>
       <c r="H54" t="n">
         <v>8962</v>
@@ -3279,13 +3279,13 @@
         <v>178.868886706413</v>
       </c>
       <c r="E55" t="n">
-        <v>18.1976301771932</v>
+        <v>36796</v>
       </c>
       <c r="F55" t="n">
-        <v>81.8023698228068</v>
+        <v>30100</v>
       </c>
       <c r="G55" t="n">
-        <v>36796</v>
+        <v>6696</v>
       </c>
       <c r="H55" t="n">
         <v>18927</v>
@@ -3323,13 +3323,13 @@
         <v>71.5347858049553</v>
       </c>
       <c r="E56" t="n">
-        <v>28.6649571716951</v>
+        <v>18329</v>
       </c>
       <c r="F56" t="n">
-        <v>71.3350428283049</v>
+        <v>13075</v>
       </c>
       <c r="G56" t="n">
-        <v>18329</v>
+        <v>5254</v>
       </c>
       <c r="H56" t="n">
         <v>9383</v>
@@ -3367,13 +3367,13 @@
         <v>615.341573288903</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>39561</v>
       </c>
       <c r="F57" t="n">
-        <v>100</v>
+        <v>13536</v>
       </c>
       <c r="G57" t="n">
-        <v>39561</v>
+        <v>26025</v>
       </c>
       <c r="H57" t="n">
         <v>20915</v>
@@ -3411,13 +3411,13 @@
         <v>36.0345848213766</v>
       </c>
       <c r="E58" t="n">
-        <v>31.7329282789592</v>
+        <v>15142</v>
       </c>
       <c r="F58" t="n">
-        <v>68.2670717210408</v>
+        <v>10337</v>
       </c>
       <c r="G58" t="n">
-        <v>15142</v>
+        <v>4805</v>
       </c>
       <c r="H58" t="n">
         <v>7763</v>
@@ -3455,13 +3455,13 @@
         <v>72.6671962311612</v>
       </c>
       <c r="E59" t="n">
-        <v>23.1064732526805</v>
+        <v>17441</v>
       </c>
       <c r="F59" t="n">
-        <v>76.8935267473195</v>
+        <v>13411</v>
       </c>
       <c r="G59" t="n">
-        <v>17441</v>
+        <v>4030</v>
       </c>
       <c r="H59" t="n">
         <v>9295</v>
@@ -3499,13 +3499,13 @@
         <v>72.3960434224666</v>
       </c>
       <c r="E60" t="n">
-        <v>24.3646408839779</v>
+        <v>38010</v>
       </c>
       <c r="F60" t="n">
-        <v>75.6353591160221</v>
+        <v>28749</v>
       </c>
       <c r="G60" t="n">
-        <v>38010</v>
+        <v>9261</v>
       </c>
       <c r="H60" t="n">
         <v>19873</v>
@@ -3543,13 +3543,13 @@
         <v>99.0930683473094</v>
       </c>
       <c r="E61" t="n">
-        <v>14.9345826429755</v>
+        <v>17503</v>
       </c>
       <c r="F61" t="n">
-        <v>85.0654173570245</v>
+        <v>14889</v>
       </c>
       <c r="G61" t="n">
-        <v>17503</v>
+        <v>2614</v>
       </c>
       <c r="H61" t="n">
         <v>9108</v>
@@ -3587,13 +3587,13 @@
         <v>231.547978862429</v>
       </c>
       <c r="E62" t="n">
-        <v>85.5276024535514</v>
+        <v>56245</v>
       </c>
       <c r="F62" t="n">
-        <v>14.4723975464486</v>
+        <v>8140</v>
       </c>
       <c r="G62" t="n">
-        <v>56245</v>
+        <v>48105</v>
       </c>
       <c r="H62" t="n">
         <v>29305</v>
@@ -3631,13 +3631,13 @@
         <v>89.9250492466342</v>
       </c>
       <c r="E63" t="n">
+        <v>31235</v>
+      </c>
+      <c r="F63" t="n">
+        <v>31235</v>
+      </c>
+      <c r="G63" t="n">
         <v>0</v>
-      </c>
-      <c r="F63" t="n">
-        <v>100</v>
-      </c>
-      <c r="G63" t="n">
-        <v>31235</v>
       </c>
       <c r="H63" t="n">
         <v>15667</v>
@@ -3675,13 +3675,13 @@
         <v>256.195494812206</v>
       </c>
       <c r="E64" t="n">
-        <v>72.8403242550748</v>
+        <v>90546</v>
       </c>
       <c r="F64" t="n">
-        <v>27.1596757449252</v>
+        <v>24592</v>
       </c>
       <c r="G64" t="n">
-        <v>90546</v>
+        <v>65954</v>
       </c>
       <c r="H64" t="n">
         <v>46484</v>
@@ -3719,13 +3719,13 @@
         <v>73.2499718253757</v>
       </c>
       <c r="E65" t="n">
+        <v>10830</v>
+      </c>
+      <c r="F65" t="n">
+        <v>10830</v>
+      </c>
+      <c r="G65" t="n">
         <v>0</v>
-      </c>
-      <c r="F65" t="n">
-        <v>100</v>
-      </c>
-      <c r="G65" t="n">
-        <v>10830</v>
       </c>
       <c r="H65" t="n">
         <v>5575</v>
@@ -3763,13 +3763,13 @@
         <v>261.894719014636</v>
       </c>
       <c r="E66" t="n">
-        <v>77.7107409925221</v>
+        <v>11768</v>
       </c>
       <c r="F66" t="n">
-        <v>22.2892590074779</v>
+        <v>2623</v>
       </c>
       <c r="G66" t="n">
-        <v>11768</v>
+        <v>9145</v>
       </c>
       <c r="H66" t="n">
         <v>6028</v>
@@ -3807,13 +3807,13 @@
         <v>143.638382626376</v>
       </c>
       <c r="E67" t="n">
-        <v>68.8152240638429</v>
+        <v>13032</v>
       </c>
       <c r="F67" t="n">
-        <v>31.1847759361572</v>
+        <v>4064</v>
       </c>
       <c r="G67" t="n">
-        <v>13032</v>
+        <v>8968</v>
       </c>
       <c r="H67" t="n">
         <v>6706</v>
@@ -3851,13 +3851,13 @@
         <v>337.532323678841</v>
       </c>
       <c r="E68" t="n">
-        <v>65.6636558203649</v>
+        <v>55134</v>
       </c>
       <c r="F68" t="n">
-        <v>34.3363441796351</v>
+        <v>18931</v>
       </c>
       <c r="G68" t="n">
-        <v>55134</v>
+        <v>36203</v>
       </c>
       <c r="H68" t="n">
         <v>28045</v>
@@ -3895,13 +3895,13 @@
         <v>53.9746364750514</v>
       </c>
       <c r="E69" t="n">
+        <v>14340</v>
+      </c>
+      <c r="F69" t="n">
+        <v>14340</v>
+      </c>
+      <c r="G69" t="n">
         <v>0</v>
-      </c>
-      <c r="F69" t="n">
-        <v>100</v>
-      </c>
-      <c r="G69" t="n">
-        <v>14340</v>
       </c>
       <c r="H69" t="n">
         <v>7322</v>
@@ -3939,13 +3939,13 @@
         <v>2191.17733762698</v>
       </c>
       <c r="E70" t="n">
-        <v>94.4522346733848</v>
+        <v>168302</v>
       </c>
       <c r="F70" t="n">
-        <v>5.54776532661525</v>
+        <v>9337</v>
       </c>
       <c r="G70" t="n">
-        <v>168302</v>
+        <v>158965</v>
       </c>
       <c r="H70" t="n">
         <v>86255</v>
@@ -3983,13 +3983,13 @@
         <v>604.836312839687</v>
       </c>
       <c r="E71" t="n">
-        <v>85.0684428593906</v>
+        <v>19067</v>
       </c>
       <c r="F71" t="n">
-        <v>14.9315571406094</v>
+        <v>2847</v>
       </c>
       <c r="G71" t="n">
-        <v>19067</v>
+        <v>16220</v>
       </c>
       <c r="H71" t="n">
         <v>9763</v>
@@ -4027,13 +4027,13 @@
         <v>17.0918469682882</v>
       </c>
       <c r="E72" t="n">
+        <v>9086</v>
+      </c>
+      <c r="F72" t="n">
+        <v>9086</v>
+      </c>
+      <c r="G72" t="n">
         <v>0</v>
-      </c>
-      <c r="F72" t="n">
-        <v>100</v>
-      </c>
-      <c r="G72" t="n">
-        <v>9086</v>
       </c>
       <c r="H72" t="n">
         <v>4675</v>
@@ -4071,13 +4071,13 @@
         <v>134.009526568541</v>
       </c>
       <c r="E73" t="n">
-        <v>72.5456672365698</v>
+        <v>11113</v>
       </c>
       <c r="F73" t="n">
-        <v>27.4543327634302</v>
+        <v>3051</v>
       </c>
       <c r="G73" t="n">
-        <v>11113</v>
+        <v>8062</v>
       </c>
       <c r="H73" t="n">
         <v>5747</v>
@@ -4115,13 +4115,13 @@
         <v>96.2022616871292</v>
       </c>
       <c r="E74" t="n">
-        <v>22.9812841312762</v>
+        <v>37722</v>
       </c>
       <c r="F74" t="n">
-        <v>77.0187158687238</v>
+        <v>29053</v>
       </c>
       <c r="G74" t="n">
-        <v>37722</v>
+        <v>8669</v>
       </c>
       <c r="H74" t="n">
         <v>19245</v>
@@ -4159,13 +4159,13 @@
         <v>734.365879157695</v>
       </c>
       <c r="E75" t="n">
-        <v>95.3992873611402</v>
+        <v>28626</v>
       </c>
       <c r="F75" t="n">
-        <v>4.60071263885978</v>
+        <v>1317</v>
       </c>
       <c r="G75" t="n">
-        <v>28626</v>
+        <v>27309</v>
       </c>
       <c r="H75" t="n">
         <v>14720</v>
@@ -4203,13 +4203,13 @@
         <v>165.845124237632</v>
       </c>
       <c r="E76" t="n">
-        <v>78.1762007302687</v>
+        <v>21362</v>
       </c>
       <c r="F76" t="n">
-        <v>21.8237992697313</v>
+        <v>4662</v>
       </c>
       <c r="G76" t="n">
-        <v>21362</v>
+        <v>16700</v>
       </c>
       <c r="H76" t="n">
         <v>11058</v>
@@ -4247,13 +4247,13 @@
         <v>342.465745079848</v>
       </c>
       <c r="E77" t="n">
-        <v>69.0427167765644</v>
+        <v>115107</v>
       </c>
       <c r="F77" t="n">
-        <v>28.5456140808118</v>
+        <v>32858</v>
       </c>
       <c r="G77" t="n">
-        <v>115107</v>
+        <v>82249</v>
       </c>
       <c r="H77" t="n">
         <v>59519</v>
@@ -4291,13 +4291,13 @@
         <v>774.414134603492</v>
       </c>
       <c r="E78" t="n">
-        <v>86.7822144476376</v>
+        <v>168369</v>
       </c>
       <c r="F78" t="n">
-        <v>13.3962836692073</v>
+        <v>22515</v>
       </c>
       <c r="G78" t="n">
-        <v>168369</v>
+        <v>145854</v>
       </c>
       <c r="H78" t="n">
         <v>88602</v>
@@ -4335,13 +4335,13 @@
         <v>134.849517910304</v>
       </c>
       <c r="E79" t="n">
+        <v>18260</v>
+      </c>
+      <c r="F79" t="n">
+        <v>18260</v>
+      </c>
+      <c r="G79" t="n">
         <v>0</v>
-      </c>
-      <c r="F79" t="n">
-        <v>100</v>
-      </c>
-      <c r="G79" t="n">
-        <v>18260</v>
       </c>
       <c r="H79" t="n">
         <v>9417</v>
@@ -4379,13 +4379,13 @@
         <v>39.6679520690589</v>
       </c>
       <c r="E80" t="n">
+        <v>7015</v>
+      </c>
+      <c r="F80" t="n">
+        <v>7015</v>
+      </c>
+      <c r="G80" t="n">
         <v>0</v>
-      </c>
-      <c r="F80" t="n">
-        <v>100</v>
-      </c>
-      <c r="G80" t="n">
-        <v>7015</v>
       </c>
       <c r="H80" t="n">
         <v>3561</v>
@@ -4423,13 +4423,13 @@
         <v>159.853296484204</v>
       </c>
       <c r="E81" t="n">
-        <v>20.0251276647483</v>
+        <v>24674</v>
       </c>
       <c r="F81" t="n">
-        <v>79.9748723352517</v>
+        <v>19733</v>
       </c>
       <c r="G81" t="n">
-        <v>24674</v>
+        <v>4941</v>
       </c>
       <c r="H81" t="n">
         <v>12614</v>
@@ -4467,13 +4467,13 @@
         <v>139.919761596279</v>
       </c>
       <c r="E82" t="n">
-        <v>77.2428253177827</v>
+        <v>38155</v>
       </c>
       <c r="F82" t="n">
-        <v>22.7571746822173</v>
+        <v>8683</v>
       </c>
       <c r="G82" t="n">
-        <v>38155</v>
+        <v>29472</v>
       </c>
       <c r="H82" t="n">
         <v>20018</v>
@@ -4511,13 +4511,13 @@
         <v>203.719663418911</v>
       </c>
       <c r="E83" t="n">
-        <v>98.7315207760108</v>
+        <v>21443</v>
       </c>
       <c r="F83" t="n">
-        <v>1.26847922398918</v>
+        <v>272</v>
       </c>
       <c r="G83" t="n">
-        <v>21443</v>
+        <v>21171</v>
       </c>
       <c r="H83" t="n">
         <v>11101</v>
@@ -4555,13 +4555,13 @@
         <v>181.024189164517</v>
       </c>
       <c r="E84" t="n">
-        <v>60.6223880081511</v>
+        <v>57906</v>
       </c>
       <c r="F84" t="n">
-        <v>39.3776119918489</v>
+        <v>22802</v>
       </c>
       <c r="G84" t="n">
-        <v>57906</v>
+        <v>35104</v>
       </c>
       <c r="H84" t="n">
         <v>30000</v>
@@ -4599,13 +4599,13 @@
         <v>45.7616146557539</v>
       </c>
       <c r="E85" t="n">
-        <v>36.8973376411952</v>
+        <v>39927</v>
       </c>
       <c r="F85" t="n">
-        <v>63.1026623588048</v>
+        <v>25195</v>
       </c>
       <c r="G85" t="n">
-        <v>39927</v>
+        <v>14732</v>
       </c>
       <c r="H85" t="n">
         <v>21028</v>

</xml_diff>